<commit_message>
Adding user guide for OSS release
</commit_message>
<xml_diff>
--- a/osc-server/techdoc/OSC_v2 5-HelpToUI-Mapping.xlsx
+++ b/osc-server/techdoc/OSC_v2 5-HelpToUI-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>UI page name</t>
   </si>
@@ -187,16 +187,13 @@
     <t>Manager Plugins</t>
   </si>
   <si>
-    <t>GUID-07FFF1BC-EA9E-426B-A247-4AF6BD12B350</t>
-  </si>
-  <si>
     <t>SDN Plugins</t>
   </si>
   <si>
-    <t>GUID-DD7DFB29-CB4F-4DD1-BFF5-21694F740D0E</t>
-  </si>
-  <si>
     <t>GUID-C6F07F61-5669-4085-AF20-07212408C984</t>
+  </si>
+  <si>
+    <t>GUID-65309889-62B2-43BE-81CE-6A4B650AAFEE</t>
   </si>
 </sst>
 </file>
@@ -588,18 +585,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.88671875" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -621,7 +618,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -632,7 +629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -643,12 +640,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -659,7 +656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -670,7 +667,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -681,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -692,7 +689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -703,7 +700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -714,7 +711,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -722,10 +719,10 @@
         <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -736,12 +733,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -752,7 +749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -763,7 +760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -771,12 +768,12 @@
         <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>39</v>
@@ -785,7 +782,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -796,7 +793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -807,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -818,7 +815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
@@ -829,7 +826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Adding user guide for OSS release (#211)
</commit_message>
<xml_diff>
--- a/osc-server/techdoc/OSC_v2 5-HelpToUI-Mapping.xlsx
+++ b/osc-server/techdoc/OSC_v2 5-HelpToUI-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>UI page name</t>
   </si>
@@ -187,16 +187,13 @@
     <t>Manager Plugins</t>
   </si>
   <si>
-    <t>GUID-07FFF1BC-EA9E-426B-A247-4AF6BD12B350</t>
-  </si>
-  <si>
     <t>SDN Plugins</t>
   </si>
   <si>
-    <t>GUID-DD7DFB29-CB4F-4DD1-BFF5-21694F740D0E</t>
-  </si>
-  <si>
     <t>GUID-C6F07F61-5669-4085-AF20-07212408C984</t>
+  </si>
+  <si>
+    <t>GUID-65309889-62B2-43BE-81CE-6A4B650AAFEE</t>
   </si>
 </sst>
 </file>
@@ -588,18 +585,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.88671875" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -621,7 +618,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -632,7 +629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -643,12 +640,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -659,7 +656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -670,7 +667,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -681,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -692,7 +689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -703,7 +700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -714,7 +711,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -722,10 +719,10 @@
         <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -736,12 +733,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -752,7 +749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -763,7 +760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -771,12 +768,12 @@
         <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>39</v>
@@ -785,7 +782,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -796,7 +793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -807,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -818,7 +815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
@@ -829,7 +826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>